<commit_message>
Fixed test excel file
</commit_message>
<xml_diff>
--- a/.test/data/test_excel.xlsx
+++ b/.test/data/test_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gupta.i/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4603505-DF4D-F149-9E97-F548803C064C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B2CD91-8144-F443-945F-05E5DCD56117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3480" yWindow="2620" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{B717BA62-2A70-7D4F-83ED-D4A6C7C15A0D}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>fwd_primer</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t>guide_5</t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
 </sst>
 </file>
@@ -574,17 +577,17 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>